<commit_message>
Presentacion sprint 1 para [06-11]
- Archivo ppt para presentar el avance del sprint 01.
- Modificaciones en administración del sprint 01
  (Cambios de términos y administración de horas) .
</commit_message>
<xml_diff>
--- a/burndown y trabajo de equipo/Boceto sprint.xlsx
+++ b/burndown y trabajo de equipo/Boceto sprint.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="2424" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="2424" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SPRINT 1 MARCELO MORALES" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="63">
   <si>
     <t>SEMANA 1</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>Jean Nail</t>
-  </si>
-  <si>
-    <t>HORAS ESTIPULADAS/REALIZADAS (SOBRANTES)</t>
   </si>
   <si>
     <t>EXTRA</t>
@@ -216,6 +213,12 @@
   <si>
     <t>IA [Terminado]</t>
   </si>
+  <si>
+    <t>HORAS ESTIPULADAS/REALIZADAS (FALTANTES)</t>
+  </si>
+  <si>
+    <t>HORAS ESTIPULADAS/REALIZADAS ((FALTANTES)</t>
+  </si>
 </sst>
 </file>
 
@@ -253,7 +256,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -313,33 +316,23 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -361,25 +354,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2058,7 +2035,7 @@
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -2095,7 +2072,7 @@
         <a:effectLst/>
       </c:spPr>
       <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
@@ -2273,7 +2250,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -2306,7 +2283,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -3615,7 +3592,7 @@
   <dimension ref="B1:P25"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3624,64 +3601,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="G1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
+      <c r="G1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="8"/>
-      <c r="J4" s="6" t="s">
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="14"/>
+      <c r="J4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="8"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="14"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="J5" s="16" t="s">
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="J5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="15" t="s">
@@ -3689,222 +3666,222 @@
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4" t="s">
+      <c r="F6" s="10"/>
+      <c r="G6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="4"/>
+      <c r="H6" s="10"/>
       <c r="J6" s="15" t="s">
         <v>1</v>
       </c>
       <c r="K6" s="15"/>
       <c r="L6" s="15"/>
-      <c r="M6" s="4" t="s">
+      <c r="M6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4" t="s">
+      <c r="N6" s="10"/>
+      <c r="O6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="P6" s="4"/>
+      <c r="P6" s="10"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8">
+        <v>2</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8">
+        <v>3</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="J7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8">
+        <v>5</v>
+      </c>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8">
+        <v>4</v>
+      </c>
+      <c r="P7" s="8"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2">
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8">
+        <v>3</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8">
         <v>2</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2">
+      <c r="H8" s="8"/>
+      <c r="J8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8">
+        <v>0</v>
+      </c>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8">
+        <v>2</v>
+      </c>
+      <c r="P8" s="8"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="J9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="N9" s="10"/>
+      <c r="O9" s="9">
         <v>3</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="J7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2">
-        <v>5</v>
-      </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2">
-        <v>4</v>
-      </c>
-      <c r="P7" s="2"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2">
-        <v>3</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2">
-        <v>2</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="J8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2">
-        <v>0</v>
-      </c>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2">
-        <v>2</v>
-      </c>
-      <c r="P8" s="2"/>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="3">
-        <v>1</v>
-      </c>
-      <c r="H9" s="3"/>
-      <c r="J9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="N9" s="4"/>
-      <c r="O9" s="3">
-        <v>3</v>
-      </c>
-      <c r="P9" s="3"/>
+      <c r="P9" s="9"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4">
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10">
         <f>SUM(E7:F11)</f>
         <v>5</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4">
+      <c r="F12" s="10"/>
+      <c r="G12" s="10">
         <f>SUM(G7:H11)</f>
         <v>6</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="J12" s="4" t="s">
+      <c r="H12" s="10"/>
+      <c r="J12" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4">
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10">
         <f>SUM(M7:N11)</f>
         <v>5</v>
       </c>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4">
+      <c r="N12" s="10"/>
+      <c r="O12" s="10">
         <f>SUM(O7:P11)</f>
         <v>9</v>
       </c>
-      <c r="P12" s="4"/>
+      <c r="P12" s="10"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="8"/>
-      <c r="J14" s="4" t="s">
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="14"/>
+      <c r="J14" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B15" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O15" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B15" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L15" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="M15" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="N15" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="O15" s="14" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.3">
@@ -3913,15 +3890,15 @@
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4" t="s">
+      <c r="F16" s="10"/>
+      <c r="G16" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H16" s="4"/>
-      <c r="J16" s="11" t="s">
+      <c r="H16" s="10"/>
+      <c r="J16" s="4" t="s">
         <v>11</v>
       </c>
       <c r="K16" s="1">
@@ -3941,20 +3918,20 @@
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2">
+      <c r="B17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8">
         <v>3</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2">
+      <c r="F17" s="8"/>
+      <c r="G17" s="8">
         <v>1</v>
       </c>
-      <c r="H17" s="2"/>
-      <c r="J17" s="11" t="s">
+      <c r="H17" s="8"/>
+      <c r="J17" s="4" t="s">
         <v>12</v>
       </c>
       <c r="K17" s="1">
@@ -3974,102 +3951,102 @@
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2">
+      <c r="B18" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8">
         <v>2</v>
       </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2">
+      <c r="F18" s="8"/>
+      <c r="G18" s="8">
         <v>3</v>
       </c>
-      <c r="H18" s="2"/>
+      <c r="H18" s="8"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B19" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4">
+      <c r="B19" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10">
         <v>1</v>
       </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="3">
+      <c r="F19" s="10"/>
+      <c r="G19" s="9">
         <v>2</v>
       </c>
-      <c r="H19" s="3"/>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2" t="s">
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2">
+      <c r="F20" s="8"/>
+      <c r="G20" s="8">
         <v>0</v>
       </c>
-      <c r="H20" s="2"/>
+      <c r="H20" s="8"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4">
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10">
         <f>SUM(E17:F24)</f>
         <v>6</v>
       </c>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4">
+      <c r="F25" s="10"/>
+      <c r="G25" s="10">
         <f>SUM(G17:H24)</f>
         <v>6</v>
       </c>
-      <c r="H25" s="4"/>
+      <c r="H25" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="80">
@@ -4097,8 +4074,6 @@
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="G19:H19"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="B14:H14"/>
     <mergeCell ref="C15:H15"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="E17:F17"/>
@@ -4107,11 +4082,11 @@
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="G16:H16"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="M11:N11"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="G11:H11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="B14:H14"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="G12:H12"/>
@@ -4124,6 +4099,8 @@
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="M10:N10"/>
     <mergeCell ref="O10:P10"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="M11:N11"/>
     <mergeCell ref="J7:L7"/>
     <mergeCell ref="M7:N7"/>
     <mergeCell ref="O7:P7"/>
@@ -4164,7 +4141,7 @@
   <dimension ref="B1:P24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4174,64 +4151,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="G1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
+      <c r="G1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
-      <c r="J3" s="6" t="s">
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="14"/>
+      <c r="J3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="8"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="14"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="J4" s="16" t="s">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="J4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="15" t="s">
@@ -4239,228 +4216,228 @@
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4" t="s">
+      <c r="F5" s="10"/>
+      <c r="G5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="4"/>
+      <c r="H5" s="10"/>
       <c r="J5" s="15" t="s">
         <v>1</v>
       </c>
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4" t="s">
+      <c r="N5" s="10"/>
+      <c r="O5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="4"/>
+      <c r="P5" s="10"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8">
+        <v>3</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8">
+        <v>3</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="J6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8">
+        <v>3</v>
+      </c>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8">
+        <v>8</v>
+      </c>
+      <c r="P6" s="8"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2">
-        <v>3</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2">
-        <v>3</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="J6" s="2" t="s">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8">
+        <v>2</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8">
+        <v>2</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="J7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2">
-        <v>3</v>
-      </c>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2">
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8">
+        <v>2</v>
+      </c>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8">
+        <v>0</v>
+      </c>
+      <c r="P7" s="8"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="9">
+        <v>1</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="J8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10">
+        <v>0</v>
+      </c>
+      <c r="N8" s="10"/>
+      <c r="O8" s="9">
+        <v>1</v>
+      </c>
+      <c r="P8" s="9"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="J9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8">
+        <v>1</v>
+      </c>
+      <c r="P9" s="8"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="P6" s="2"/>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2">
-        <v>2</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2">
-        <v>2</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="J7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2">
-        <v>2</v>
-      </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2">
-        <v>0</v>
-      </c>
-      <c r="P7" s="2"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="3">
-        <v>1</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="J8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4">
-        <v>0</v>
-      </c>
-      <c r="N8" s="4"/>
-      <c r="O8" s="3">
-        <v>1</v>
-      </c>
-      <c r="P8" s="3"/>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="J9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2">
-        <v>1</v>
-      </c>
-      <c r="P9" s="2"/>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10">
         <f>SUM(E6:F10)</f>
         <v>5</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4">
+      <c r="F11" s="10"/>
+      <c r="G11" s="10">
         <f>SUM(G6:H10)</f>
         <v>6</v>
       </c>
-      <c r="H11" s="4"/>
-      <c r="J11" s="4" t="s">
+      <c r="H11" s="10"/>
+      <c r="J11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4">
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10">
         <f>SUM(M6:N10)</f>
         <v>5</v>
       </c>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4">
+      <c r="N11" s="10"/>
+      <c r="O11" s="10">
         <f>SUM(O6:P10)</f>
         <v>10</v>
       </c>
-      <c r="P11" s="4"/>
+      <c r="P11" s="10"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="8"/>
-      <c r="J13" s="12" t="s">
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="14"/>
+      <c r="J13" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B14" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O14" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B14" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L14" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="M14" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="N14" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="O14" s="14" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.3">
@@ -4469,15 +4446,15 @@
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4" t="s">
+      <c r="F15" s="10"/>
+      <c r="G15" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="4"/>
-      <c r="J15" s="11" t="s">
+      <c r="H15" s="10"/>
+      <c r="J15" s="4" t="s">
         <v>11</v>
       </c>
       <c r="K15" s="1">
@@ -4498,20 +4475,20 @@
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B16" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2">
+      <c r="B16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8">
         <v>5</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2">
+      <c r="F16" s="8"/>
+      <c r="G16" s="8">
         <v>4</v>
       </c>
-      <c r="H16" s="2"/>
-      <c r="J16" s="11" t="s">
+      <c r="H16" s="8"/>
+      <c r="J16" s="4" t="s">
         <v>12</v>
       </c>
       <c r="K16" s="1">
@@ -4531,90 +4508,90 @@
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4" t="s">
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="3">
+      <c r="F18" s="10"/>
+      <c r="G18" s="9">
         <v>2</v>
       </c>
-      <c r="H18" s="3"/>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4">
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10">
         <f>SUM(E16:F23)</f>
         <v>5</v>
       </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4">
+      <c r="F24" s="10"/>
+      <c r="G24" s="10">
         <f>SUM(G16:H23)</f>
         <v>6</v>
       </c>
-      <c r="H24" s="4"/>
+      <c r="H24" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="80">
@@ -4709,7 +4686,7 @@
   <dimension ref="B1:P24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:K2"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4718,64 +4695,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="G1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
+      <c r="G1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
-      <c r="J3" s="6" t="s">
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="14"/>
+      <c r="J3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="8"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="14"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="J4" s="16" t="s">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="J4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="15" t="s">
@@ -4783,204 +4760,204 @@
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4" t="s">
+      <c r="F5" s="10"/>
+      <c r="G5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="4"/>
+      <c r="H5" s="10"/>
       <c r="J5" s="15" t="s">
         <v>1</v>
       </c>
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4" t="s">
+      <c r="N5" s="10"/>
+      <c r="O5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="4"/>
+      <c r="P5" s="10"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8">
+        <v>5</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8">
+        <v>5</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="J6" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2">
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8">
         <v>5</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2">
+      <c r="N6" s="8"/>
+      <c r="O6" s="8">
         <v>5</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="J6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2">
-        <v>5</v>
-      </c>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2">
-        <v>5</v>
-      </c>
-      <c r="P6" s="2"/>
+      <c r="P6" s="8"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="J8" s="3" t="s">
+      <c r="F8" s="10"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="J8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10">
         <f>SUM(E6:F10)</f>
         <v>5</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4">
+      <c r="F11" s="10"/>
+      <c r="G11" s="10">
         <f>SUM(G6:H10)</f>
         <v>5</v>
       </c>
-      <c r="H11" s="4"/>
-      <c r="J11" s="4" t="s">
+      <c r="H11" s="10"/>
+      <c r="J11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4">
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10">
         <f>SUM(M6:N10)</f>
         <v>5</v>
       </c>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4">
+      <c r="N11" s="10"/>
+      <c r="O11" s="10">
         <f>SUM(O6:P10)</f>
         <v>5</v>
       </c>
-      <c r="P11" s="4"/>
+      <c r="P11" s="10"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="8"/>
-      <c r="J13" s="12" t="s">
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="14"/>
+      <c r="J13" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B14" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O14" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B14" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L14" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="M14" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="N14" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="O14" s="14" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.3">
@@ -4989,15 +4966,15 @@
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4" t="s">
+      <c r="F15" s="10"/>
+      <c r="G15" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="4"/>
-      <c r="J15" s="11" t="s">
+      <c r="H15" s="10"/>
+      <c r="J15" s="4" t="s">
         <v>11</v>
       </c>
       <c r="K15" s="1">
@@ -5018,20 +4995,20 @@
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2">
+      <c r="B16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8">
         <v>0</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2">
+      <c r="F16" s="8"/>
+      <c r="G16" s="8">
         <v>2</v>
       </c>
-      <c r="H16" s="2"/>
-      <c r="J16" s="11" t="s">
+      <c r="H16" s="8"/>
+      <c r="J16" s="4" t="s">
         <v>12</v>
       </c>
       <c r="K16" s="1">
@@ -5051,102 +5028,102 @@
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8">
+        <v>3</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8">
+        <v>3</v>
+      </c>
+      <c r="H17" s="8"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10">
+        <v>0</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="9">
+        <v>3</v>
+      </c>
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2">
-        <v>3</v>
-      </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2">
-        <v>3</v>
-      </c>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4">
-        <v>0</v>
-      </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="3">
-        <v>3</v>
-      </c>
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2">
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8">
         <v>2</v>
       </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2">
+      <c r="F19" s="8"/>
+      <c r="G19" s="8">
         <v>2</v>
       </c>
-      <c r="H19" s="2"/>
+      <c r="H19" s="8"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4">
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10">
         <f>SUM(E16:F23)</f>
         <v>5</v>
       </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4">
+      <c r="F24" s="10"/>
+      <c r="G24" s="10">
         <f>SUM(G16:H23)</f>
         <v>10</v>
       </c>
-      <c r="H24" s="4"/>
+      <c r="H24" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="80">
@@ -5240,8 +5217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5250,64 +5227,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
-      <c r="J3" s="6" t="s">
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="14"/>
+      <c r="J3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="8"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="14"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="J4" s="16" t="s">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="J4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="15" t="s">
@@ -5315,222 +5292,222 @@
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4" t="s">
+      <c r="F5" s="10"/>
+      <c r="G5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="4"/>
+      <c r="H5" s="10"/>
       <c r="J5" s="15" t="s">
         <v>1</v>
       </c>
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4" t="s">
+      <c r="N5" s="10"/>
+      <c r="O5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="4"/>
+      <c r="P5" s="10"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8">
+        <v>2</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8">
+        <v>4</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="J6" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8">
+        <v>2</v>
+      </c>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8">
+        <v>2</v>
+      </c>
+      <c r="P6" s="8"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B7" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8">
+        <v>3</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8">
+        <v>4</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="J7" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8">
+        <v>3</v>
+      </c>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8">
         <v>2</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2">
-        <v>4</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="J6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2">
+      <c r="P7" s="8"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="9">
+        <v>1</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="J8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="N8" s="10"/>
+      <c r="O8" s="9">
         <v>2</v>
       </c>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2">
-        <v>2</v>
-      </c>
-      <c r="P6" s="2"/>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2">
-        <v>3</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2">
-        <v>4</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="J7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2">
-        <v>3</v>
-      </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2">
-        <v>2</v>
-      </c>
-      <c r="P7" s="2"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="3">
-        <v>1</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="J8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="N8" s="4"/>
-      <c r="O8" s="3">
-        <v>2</v>
-      </c>
-      <c r="P8" s="3"/>
+      <c r="P8" s="9"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10">
         <f>SUM(E6:F10)</f>
         <v>5</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4">
+      <c r="F11" s="10"/>
+      <c r="G11" s="10">
         <f>SUM(G6:H10)</f>
         <v>9</v>
       </c>
-      <c r="H11" s="4"/>
-      <c r="J11" s="4" t="s">
+      <c r="H11" s="10"/>
+      <c r="J11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4">
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10">
         <f>SUM(M6:N10)</f>
         <v>5</v>
       </c>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4">
+      <c r="N11" s="10"/>
+      <c r="O11" s="10">
         <f>SUM(O6:P10)</f>
         <v>6</v>
       </c>
-      <c r="P11" s="4"/>
+      <c r="P11" s="10"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="8"/>
-      <c r="J13" s="12" t="s">
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="14"/>
+      <c r="J13" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B14" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O14" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B14" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L14" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="M14" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="N14" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="O14" s="14" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.3">
@@ -5539,15 +5516,15 @@
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4" t="s">
+      <c r="F15" s="10"/>
+      <c r="G15" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="4"/>
-      <c r="J15" s="11" t="s">
+      <c r="H15" s="10"/>
+      <c r="J15" s="4" t="s">
         <v>11</v>
       </c>
       <c r="K15" s="1">
@@ -5568,20 +5545,20 @@
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B16" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2">
+      <c r="B16" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8">
         <v>5</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2">
+      <c r="F16" s="8"/>
+      <c r="G16" s="8">
         <v>4</v>
       </c>
-      <c r="H16" s="2"/>
-      <c r="J16" s="11" t="s">
+      <c r="H16" s="8"/>
+      <c r="J16" s="4" t="s">
         <v>12</v>
       </c>
       <c r="K16" s="1">
@@ -5601,91 +5578,91 @@
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="J17" s="17"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="J17" s="7"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4" t="s">
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="3">
+      <c r="F18" s="10"/>
+      <c r="G18" s="9">
         <v>2</v>
       </c>
-      <c r="H18" s="3"/>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4">
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10">
         <f>SUM(E16:F23)</f>
         <v>5</v>
       </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4">
+      <c r="F24" s="10"/>
+      <c r="G24" s="10">
         <f>SUM(G16:H23)</f>
         <v>6</v>
       </c>
-      <c r="H24" s="4"/>
+      <c r="H24" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="80">
@@ -5779,71 +5756,71 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="G1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
+      <c r="G1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
-      <c r="J3" s="6" t="s">
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="14"/>
+      <c r="J3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="8"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="14"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="J4" s="16" t="s">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="J4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="15" t="s">
@@ -5851,212 +5828,212 @@
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4" t="s">
+      <c r="F5" s="10"/>
+      <c r="G5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="4"/>
+      <c r="H5" s="10"/>
       <c r="J5" s="15" t="s">
         <v>1</v>
       </c>
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4" t="s">
+      <c r="N5" s="10"/>
+      <c r="O5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="4"/>
+      <c r="P5" s="10"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8">
+        <v>5</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8">
+        <v>15</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="J6" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2">
-        <v>5</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2">
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8">
+        <v>2</v>
+      </c>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8">
+        <v>3</v>
+      </c>
+      <c r="P6" s="8"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="J7" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8">
+        <v>3</v>
+      </c>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8">
+        <v>3</v>
+      </c>
+      <c r="P7" s="8"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="J8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="J6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2">
-        <v>2</v>
-      </c>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2">
-        <v>3</v>
-      </c>
-      <c r="P6" s="2"/>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="J7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2">
-        <v>3</v>
-      </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2">
-        <v>3</v>
-      </c>
-      <c r="P7" s="2"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4" t="s">
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="J8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="N8" s="4"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10">
         <f>SUM(E6:F10)</f>
         <v>5</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4">
+      <c r="F11" s="10"/>
+      <c r="G11" s="10">
         <f>SUM(G6:H10)</f>
         <v>15</v>
       </c>
-      <c r="H11" s="4"/>
-      <c r="J11" s="4" t="s">
+      <c r="H11" s="10"/>
+      <c r="J11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4">
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10">
         <f>SUM(M6:N10)</f>
         <v>5</v>
       </c>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4">
+      <c r="N11" s="10"/>
+      <c r="O11" s="10">
         <f>SUM(O6:P10)</f>
         <v>6</v>
       </c>
-      <c r="P11" s="4"/>
+      <c r="P11" s="10"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="8"/>
-      <c r="J13" s="12" t="s">
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="14"/>
+      <c r="J13" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B14" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O14" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B14" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L14" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="M14" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="N14" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="O14" s="14" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.3">
@@ -6065,15 +6042,15 @@
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4" t="s">
+      <c r="F15" s="10"/>
+      <c r="G15" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="4"/>
-      <c r="J15" s="11" t="s">
+      <c r="H15" s="10"/>
+      <c r="J15" s="4" t="s">
         <v>11</v>
       </c>
       <c r="K15" s="1">
@@ -6094,20 +6071,20 @@
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B16" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2">
+      <c r="B16" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8">
         <v>3</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2">
+      <c r="F16" s="8"/>
+      <c r="G16" s="8">
         <v>3</v>
       </c>
-      <c r="H16" s="2"/>
-      <c r="J16" s="11" t="s">
+      <c r="H16" s="8"/>
+      <c r="J16" s="4" t="s">
         <v>12</v>
       </c>
       <c r="K16" s="1">
@@ -6127,92 +6104,92 @@
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2">
+      <c r="B17" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8">
         <v>2</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2">
+      <c r="F17" s="8"/>
+      <c r="G17" s="8">
         <v>3</v>
       </c>
-      <c r="H17" s="2"/>
+      <c r="H17" s="8"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="3"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4" t="s">
+      <c r="B18" s="9"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4">
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10">
         <f>SUM(E16:F23)</f>
         <v>5</v>
       </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4">
+      <c r="F24" s="10"/>
+      <c r="G24" s="10">
         <f>SUM(G16:H23)</f>
         <v>6</v>
       </c>
-      <c r="H24" s="4"/>
+      <c r="H24" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="80">
@@ -6306,8 +6283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6318,103 +6295,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+    </row>
+    <row r="2" spans="2:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B4" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-    </row>
-    <row r="2" spans="2:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="L4" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B5" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="L4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="4" t="s">
+      <c r="F5" s="3"/>
+      <c r="G5" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="M5" s="10"/>
+      <c r="N5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="M5" s="4"/>
-      <c r="N5" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="O5" s="11" t="s">
+      <c r="O5" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="2"/>
+      <c r="B6" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="8"/>
       <c r="D6" s="1">
         <v>25</v>
       </c>
       <c r="E6" s="1">
         <v>41</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" s="2"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="8"/>
       <c r="I6" s="1">
         <v>25</v>
       </c>
       <c r="J6" s="1">
         <v>36</v>
       </c>
-      <c r="L6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="M6" s="2"/>
+      <c r="L6" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="M6" s="8"/>
       <c r="N6" s="1">
         <v>25</v>
       </c>
@@ -6423,31 +6400,31 @@
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="1">
         <v>25</v>
       </c>
       <c r="E7" s="1">
         <v>41</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="4" t="s">
+      <c r="F7" s="3"/>
+      <c r="G7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="4"/>
+      <c r="H7" s="10"/>
       <c r="I7" s="1">
         <v>25</v>
       </c>
       <c r="J7" s="1">
         <v>36</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="4"/>
+      <c r="M7" s="10"/>
       <c r="N7" s="1">
         <v>25</v>
       </c>
@@ -6456,45 +6433,45 @@
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="14"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="E10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="F10" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="4" t="s">
+      <c r="H10" s="3"/>
+      <c r="I10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="4"/>
+      <c r="J10" s="10"/>
       <c r="K10" s="1">
         <v>75</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="1">
@@ -6510,18 +6487,18 @@
       <c r="F11" s="1">
         <v>0</v>
       </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="4" t="s">
+      <c r="H11" s="3"/>
+      <c r="I11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="4"/>
+      <c r="J11" s="10"/>
       <c r="K11" s="1">
         <f>E7+J7+O7</f>
         <v>127</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="1">
@@ -6536,11 +6513,11 @@
       <c r="F12" s="1">
         <v>0</v>
       </c>
-      <c r="H12" s="10"/>
-      <c r="I12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J12" s="4"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="10"/>
       <c r="K12" s="1">
         <v>42</v>
       </c>

</xml_diff>